<commit_message>
Added description tab to AHLE scenario file
</commit_message>
<xml_diff>
--- a/Ethiopia Workspace/AHLE scenario parameters.xlsx
+++ b/Ethiopia Workspace/AHLE scenario parameters.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\First Analytics\Clients\University of Liverpool\GBADs Github\GBADsLiverpool\Ethiopia Workspace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6667DB8-6FEC-462F-B778-99F107B2E5AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A882648-BFE5-4A8E-87D7-F8B0B670CC62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="14292" windowWidth="23256" windowHeight="12720" xr2:uid="{7B09E95E-6D5F-461A-A5DC-5B71F2D22658}"/>
+    <workbookView xWindow="0" yWindow="2100" windowWidth="28800" windowHeight="15900" activeTab="1" xr2:uid="{7B09E95E-6D5F-461A-A5DC-5B71F2D22658}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="About" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -93,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1424" uniqueCount="364">
   <si>
     <t># Initial population</t>
   </si>
@@ -1164,6 +1165,27 @@
   </si>
   <si>
     <t>rpert(10000, 1000, 1300, 1204)</t>
+  </si>
+  <si>
+    <t>The first row must contain column names</t>
+  </si>
+  <si>
+    <t>Don't change the names of the first or second columns ('AHLE Parameter' and 'Notes')</t>
+  </si>
+  <si>
+    <t>The AHLE Parameter column must contain the names of the parameters as they appear in the function definition.  They are case-sensitive.  Rows with blanks and rows containing pound signs (#) are ignored.</t>
+  </si>
+  <si>
+    <t>The Notes column is ignored so you can write whatever you want there</t>
+  </si>
+  <si>
+    <t>All other columns are interpreted as scenarios, so must be complete (contain a value for every AHLE parameter).  You can name these columns whatever you want; the names will be used for the output files.</t>
+  </si>
+  <si>
+    <t>Double check your parameter values, especially for missing parenthesis as these will cause errors (e.g. rpert(10000, 0.52, 0.67, 0.60)).  I fixed the missing parenthesis in the current spreadsheet.</t>
+  </si>
+  <si>
+    <t>Rules for this to be read by the program</t>
   </si>
 </sst>
 </file>
@@ -1176,7 +1198,7 @@
     <numFmt numFmtId="166" formatCode="0.00000"/>
     <numFmt numFmtId="167" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1231,6 +1253,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1292,7 +1321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1337,6 +1366,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1352,10 +1385,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1657,7 +1686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCDE79AB-593E-49D8-BC0E-644D5608E970}">
   <dimension ref="A1:BB121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="Q22" sqref="Q22"/>
     </sheetView>
@@ -12231,4 +12260,54 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3D08064-68C3-4BB0-A64D-3A606C4D4B6B}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>362</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Calculate AHLE from age*sex specific scenarios
</commit_message>
<xml_diff>
--- a/Ethiopia Workspace/AHLE scenario parameters.xlsx
+++ b/Ethiopia Workspace/AHLE scenario parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\First Analytics\Clients\University of Liverpool\GBADs Github\GBADsLiverpool\Ethiopia Workspace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A882648-BFE5-4A8E-87D7-F8B0B670CC62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF414E6-C5BE-4755-9567-71C40D247D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2100" windowWidth="28800" windowHeight="15900" activeTab="1" xr2:uid="{7B09E95E-6D5F-461A-A5DC-5B71F2D22658}"/>
+    <workbookView xWindow="-108" yWindow="14292" windowWidth="23256" windowHeight="12720" xr2:uid="{7B09E95E-6D5F-461A-A5DC-5B71F2D22658}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1424" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="364">
   <si>
     <t># Initial population</t>
   </si>
@@ -1686,9 +1686,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCDE79AB-593E-49D8-BC0E-644D5608E970}">
   <dimension ref="A1:BB121"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q22" sqref="Q22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AM1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AP38" sqref="AP38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5579,6 +5579,9 @@
       <c r="AO37" t="s">
         <v>131</v>
       </c>
+      <c r="AP37" s="22" t="s">
+        <v>131</v>
+      </c>
       <c r="AQ37" t="s">
         <v>131</v>
       </c>
@@ -12266,7 +12269,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3D08064-68C3-4BB0-A64D-3A606C4D4B6B}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>

</xml_diff>